<commit_message>
Fixed bug in deleting blank zero-index row in WIDTH, DEPTH, and AREA 2d arrays in Save_Results
</commit_message>
<xml_diff>
--- a/OUTPUTS/av_CreekMorphometry.xlsx
+++ b/OUTPUTS/av_CreekMorphometry.xlsx
@@ -565,9 +565,15 @@
       <c r="E4" t="n">
         <v>13.21739130434783</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>98.68130522039117</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12.41175809502602</v>
+      </c>
+      <c r="H4" t="n">
+        <v>27738.68352655321</v>
+      </c>
       <c r="I4" t="n">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Debugged data type for straight distance array STRAIGHTDIST. Fixed the reversed Strahler order column of the summary table in Save_Results.py. It was originally backwards.
</commit_message>
<xml_diff>
--- a/OUTPUTS/av_CreekMorphometry.xlsx
+++ b/OUTPUTS/av_CreekMorphometry.xlsx
@@ -499,7 +499,7 @@
         <v>9.130434782608695</v>
       </c>
       <c r="E2" t="n">
-        <v>9.130434782608695</v>
+        <v>0.8825501377182884</v>
       </c>
       <c r="F2" t="n">
         <v>5.247265419067052</v>
@@ -511,10 +511,10 @@
         <v>1.027178528479168</v>
       </c>
       <c r="I2" t="n">
-        <v>23</v>
+        <v>235.2063318150511</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>10.22636225282831</v>
       </c>
     </row>
     <row r="3">
@@ -531,7 +531,7 @@
         <v>128.6666666666667</v>
       </c>
       <c r="E3" t="n">
-        <v>16.78260869565218</v>
+        <v>0.1251035512923761</v>
       </c>
       <c r="F3" t="n">
         <v>53.74007416700906</v>
@@ -543,10 +543,10 @@
         <v>8641.387722089887</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>382.493470473173</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>127.4978234910577</v>
       </c>
     </row>
     <row r="4">
@@ -563,7 +563,7 @@
         <v>304</v>
       </c>
       <c r="E4" t="n">
-        <v>13.21739130434783</v>
+        <v>0.05987834989280399</v>
       </c>
       <c r="F4" t="n">
         <v>98.68130522039117</v>
@@ -575,10 +575,10 @@
         <v>27738.68352655321</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>220.7374005464412</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>220.7374005464412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated plots to have correct axis orientations.
</commit_message>
<xml_diff>
--- a/OUTPUTS/av_CreekMorphometry.xlsx
+++ b/OUTPUTS/av_CreekMorphometry.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Fixed error in sinuous length calculation and summary calculations. Fixed a small bug in if statements for creek ordering. Added some nicer filenaming and saving conventions.
</commit_message>
<xml_diff>
--- a/OUTPUTS/av_CreekMorphometry.xlsx
+++ b/OUTPUTS/av_CreekMorphometry.xlsx
@@ -487,34 +487,34 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
         <v>23</v>
       </c>
       <c r="C2" t="n">
-        <v>210</v>
+        <v>250.1787155501902</v>
       </c>
       <c r="D2" t="n">
-        <v>9.130434782608695</v>
+        <v>10.87733545870392</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8825501377182884</v>
+        <v>1.053701939707178</v>
       </c>
       <c r="F2" t="n">
-        <v>5.247265419067052</v>
+        <v>5.019123444325006</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4233862981200218</v>
+        <v>0.40497819820176</v>
       </c>
       <c r="H2" t="n">
-        <v>1.027178528479168</v>
+        <v>0.6252391042916673</v>
       </c>
       <c r="I2" t="n">
-        <v>235.2063318150511</v>
+        <v>234.276888520289</v>
       </c>
       <c r="J2" t="n">
-        <v>10.22636225282831</v>
+        <v>10.18595167479518</v>
       </c>
     </row>
     <row r="3">
@@ -525,13 +525,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>386</v>
+        <v>446.4751801064722</v>
       </c>
       <c r="D3" t="n">
-        <v>128.6666666666667</v>
+        <v>148.8250600354907</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1251035512923761</v>
+        <v>1.136229726332538</v>
       </c>
       <c r="F3" t="n">
         <v>53.74007416700906</v>
@@ -551,19 +551,19 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>304</v>
+        <v>370.6883835420692</v>
       </c>
       <c r="D4" t="n">
-        <v>304</v>
+        <v>370.6883835420692</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05987834989280399</v>
+        <v>1.679318423721673</v>
       </c>
       <c r="F4" t="n">
         <v>98.68130522039117</v>

</xml_diff>